<commit_message>
NLGI NAS rates upated
</commit_message>
<xml_diff>
--- a/Input/NLGI_NAS/benefits.xlsx
+++ b/Input/NLGI_NAS/benefits.xlsx
@@ -304,7 +304,7 @@
     <t xml:space="preserve">NLGI_Nas</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-12-06</t>
+    <t xml:space="preserve">2024-05-01</t>
   </si>
   <si>
     <t xml:space="preserve">Consultations 20% with AED 50 max, nil co-pay on all OP services/Nil/Nil</t>
@@ -313,7 +313,7 @@
     <t xml:space="preserve">Annually</t>
   </si>
   <si>
-    <t xml:space="preserve">UAE</t>
+    <t xml:space="preserve">NE/Dubai</t>
   </si>
   <si>
     <t xml:space="preserve">Plan 2</t>
@@ -357,7 +357,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -384,11 +384,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -433,7 +428,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,10 +447,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -481,16 +472,16 @@
   </sheetPr>
   <dimension ref="A1:BK6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BA3" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BK3" activeCellId="0" sqref="BK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="40.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="34.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="15.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="59.01"/>
@@ -679,7 +670,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -829,7 +820,7 @@
       <c r="BF2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BG2" s="5" t="s">
         <v>91</v>
       </c>
       <c r="BH2" s="0" t="s">

</xml_diff>